<commit_message>
Added checks that xs are sorted
</commit_message>
<xml_diff>
--- a/LAMBDA Cubic Spline v000.xlsx
+++ b/LAMBDA Cubic Spline v000.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yake\Documents\GitHub\excel-lambda-cubic-spline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FAD979-E882-4288-B46A-8C6B591BB588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B462031-9A31-4E9A-91E8-B3A5D5703E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Python Code" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CUBIC_SPLINE_POLATION">_xlfn.LAMBDA(_xlpm.xs,_xlpm.ys,_xlpm.desired_xs,_xlpm.end_type,_xlfn.LET(_xlpm.xs_rows,ROWS(_xlpm.xs),_xlpm.xs_cols,COLUMNS(_xlpm.xs),_xlpm.ys_rows,ROWS(_xlpm.ys),_xlpm.ys_cols,COLUMNS(_xlpm.ys),_xlpm.desired_xs_rows,ROWS(_xlpm.desired_xs),_xlpm.desired_xs_cols, COLUMNS(_xlpm.desired_xs),_xlfn.IFS(_xlfn.ISOMITTED(_xlpm.xs),"Missing argument xs",_xlfn.ISOMITTED(_xlpm.ys),"Missing argument ys",_xlfn.ISOMITTED(_xlpm.desired_xs),"Missing argument desired_xs",_xlfn.ISOMITTED(_xlpm.end_type),"Missing argument end_type",AND(_xlpm.xs_rows&gt;1,_xlpm.xs_cols&gt;1),"Argument xs is a matrix, expecting a vector",AND(_xlpm.ys_rows&gt;1,_xlpm.ys_cols&gt;1),"Argument ys is a matrix, expecting a vector",AND(_xlpm.desired_xs_rows&gt;1,_xlpm.desired_xs_cols&gt;1),"Argument desired_xs is a matrix, expecting a vector",_xlpm.xs_rows+_xlpm.xs_cols&lt;4,"Argument xs is too small, need to be a vector with at least 3 elements",_xlpm.ys_rows+_xlpm.ys_cols&lt;4,"Argument ys is too small, need to be a vector with at least 3 elements",_xlfn.XOR(_xlpm.xs_rows=1,_xlpm.ys_rows=1),"Arguments xs and ys must be both column vectors or both row vectors, not mixed",_xlpm.xs_rows+_xlpm.xs_cols&lt;&gt;_xlpm.ys_rows+_xlpm.ys_cols,"Argument vectors xs and ys must both have the same length",AND(_xlfn.XOR(_xlpm.xs_rows=1,_xlpm.desired_xs_rows=1),_xlpm.desired_xs_rows+_xlpm.desired_xs_cols&gt;2),"Arguments xs and desired xs must be both column vectors or both row vectors, not a mix",AND(_xlpm.end_type&lt;&gt;0,_xlpm.end_type&lt;&gt;1),"Argument end_type must be either 0 for Natural or 1 for Not-a-Knot, no other values permitted",TRUE,IF(_xlpm.xs_cols=1,INTERNAL_CUBIC_SPLINE_POLATION(_xlpm.xs,_xlpm.ys,_xlpm.desired_xs,_xlpm.end_type),TRANSPOSE(INTERNAL_CUBIC_SPLINE_POLATION(TRANSPOSE(_xlpm.xs),TRANSPOSE(_xlpm.ys),TRANSPOSE(_xlpm.desired_xs),_xlpm.end_type))))))</definedName>
+    <definedName name="CUBIC_SPLINE_POLATION">_xlfn.LAMBDA(_xlpm.xs,_xlpm.ys,_xlpm.desired_xs,_xlpm.end_type,_xlfn.LET(_xlpm.xs_rows,ROWS(_xlpm.xs),_xlpm.xs_cols,COLUMNS(_xlpm.xs),_xlpm.ys_rows,ROWS(_xlpm.ys),_xlpm.ys_cols,COLUMNS(_xlpm.ys),_xlpm.desired_xs_rows,ROWS(_xlpm.desired_xs),_xlpm.desired_xs_cols, COLUMNS(_xlpm.desired_xs),_xlpm.dxs,IF(_xlpm.xs_cols=1,_xlfn.DROP(_xlpm.xs,1,)-_xlfn.TAKE(_xlpm.xs,_xlpm.xs_rows-1,),_xlfn.DROP(_xlpm.xs,,1)-_xlfn.TAKE(_xlpm.xs,,_xlpm.xs_cols-1)),_xlfn.IFS(_xlfn.ISOMITTED(_xlpm.xs),"Missing argument xs",_xlfn.ISOMITTED(_xlpm.ys),"Missing argument ys",_xlfn.ISOMITTED(_xlpm.desired_xs),"Missing argument desired_xs",_xlfn.ISOMITTED(_xlpm.end_type),"Missing argument end_type",AND(_xlpm.xs_rows&gt;1,_xlpm.xs_cols&gt;1),"Argument xs is a matrix, expecting a vector",AND(_xlpm.ys_rows&gt;1,_xlpm.ys_cols&gt;1),"Argument ys is a matrix, expecting a vector",AND(_xlpm.desired_xs_rows&gt;1,_xlpm.desired_xs_cols&gt;1),"Argument desired_xs is a matrix, expecting a vector",_xlpm.xs_rows+_xlpm.xs_cols&lt;4,"Argument xs is too small, need to be a vector with at least 3 elements",_xlpm.ys_rows+_xlpm.ys_cols&lt;4,"Argument ys is too small, need to be a vector with at least 3 elements",_xlfn.XOR(_xlpm.xs_rows=1,_xlpm.ys_rows=1),"Arguments xs and ys must be both column vectors or both row vectors, not mixed",_xlpm.xs_rows+_xlpm.xs_cols&lt;&gt;_xlpm.ys_rows+_xlpm.ys_cols,"Argument vectors xs and ys must both have the same length",AND(_xlfn.XOR(_xlpm.xs_rows=1,_xlpm.desired_xs_rows=1),_xlpm.desired_xs_rows+_xlpm.desired_xs_cols&gt;2),"Arguments xs and desired xs must be both column vectors or both row vectors, not a mix",AND(_xlpm.end_type&lt;&gt;0,_xlpm.end_type&lt;&gt;1),"Argument end_type must be either 0 for Natural or 1 for Not-a-Knot, no other values permitted",OR(_xlpm.dxs&lt;0),"Argument xs must be in increasing order",TRUE,IF(_xlpm.xs_cols=1,INTERNAL_CUBIC_SPLINE_POLATION(_xlpm.xs,_xlpm.ys,_xlpm.desired_xs,_xlpm.end_type),TRANSPOSE(INTERNAL_CUBIC_SPLINE_POLATION(TRANSPOSE(_xlpm.xs),TRANSPOSE(_xlpm.ys),TRANSPOSE(_xlpm.desired_xs),_xlpm.end_type))))))</definedName>
     <definedName name="INTERNAL_CUBIC_SPLINE_POLATION">_xlfn.LAMBDA(_xlpm.xs,_xlpm.ys,_xlpm.desired_xs,_xlpm.end_type,_xlfn.LET(_xlpm.n,ROWS(_xlpm.xs)-1,_xlpm.dxs,_xlfn.DROP(_xlpm.xs,1,)-_xlfn.TAKE(_xlpm.xs,_xlpm.n,),_xlpm.dys,_xlfn.DROP(_xlpm.ys,1,)-_xlfn.TAKE(_xlpm.ys,_xlpm.n,),_xlpm.recip_dxs,1/_xlpm.dxs,_xlpm.recip_dxs_sq,_xlpm.recip_dxs*_xlpm.recip_dxs,_xlpm.dy_recip_dxs_sq,_xlpm.dys*_xlpm.recip_dxs_sq,_xlpm.matrix_f,_xlfn.MAKEARRAY(_xlpm.n+1,_xlpm.n+1,_xlfn.LAMBDA(_xlpm.row,_xlpm.col,_xlfn.LET(_xlpm.other_rows,_xlfn.IFS(_xlpm.col=_xlpm.row-1,INDEX(_xlpm.recip_dxs,_xlpm.row-1,1),_xlpm.col=_xlpm.row,2*(INDEX(_xlpm.recip_dxs,_xlpm.row-1,1)+INDEX(_xlpm.recip_dxs,_xlpm.row,1)),_xlpm.col=_xlpm.row+1,INDEX(_xlpm.recip_dxs,_xlpm.row,1),TRUE,0),IF(OR(_xlpm.row=1,_xlpm.row=_xlpm.n+1),INTERNAL_SPLINE_MATRIX_TOP_BOTTOM(_xlpm.end_type,_xlpm.row,_xlpm.col,_xlpm.recip_dxs,_xlpm.recip_dxs_sq),_xlpm.other_rows)))),_xlpm.yi_over_xi2_times3,_xlpm.dy_recip_dxs_sq*3,_xlpm.vec_g_top,INTERNAL_SPLINE_VECTOR_TOP_BOTTOM(_xlpm.end_type,1,_xlpm.recip_dxs,_xlpm.dy_recip_dxs_sq),_xlpm.vec_g_bottom,INTERNAL_SPLINE_VECTOR_TOP_BOTTOM(_xlpm.end_type,_xlpm.n+1,_xlpm.recip_dxs,_xlpm.dy_recip_dxs_sq),_xlpm.vector_g,_xlfn.VSTACK(_xlpm.vec_g_top,_xlfn.DROP(_xlpm.yi_over_xi2_times3,1,)+_xlfn.TAKE(_xlpm.yi_over_xi2_times3,_xlpm.n-1,),_xlpm.vec_g_bottom),_xlpm.ks,MMULT(MINVERSE(_xlpm.matrix_f),_xlpm.vector_g),_xlpm.as,_xlfn.TAKE(_xlpm.ks,_xlpm.n,)*_xlpm.dxs-_xlpm.dys,_xlpm.bs,-_xlfn.DROP(_xlpm.ks,1,)*_xlpm.dxs+_xlpm.dys,_xlpm.min_xi,INDEX(_xlpm.xs,1,1),_xlpm.max_xi,INDEX(_xlpm.xs,_xlpm.n+1,1),_xlpm.calc_idxs,_xlfn.IFS(_xlpm.desired_xs&lt;_xlpm.min_xi,1,_xlpm.desired_xs&gt;=_xlpm.max_xi,_xlpm.n,TRUE,_xlfn.XMATCH(_xlpm.desired_xs,_xlpm.xs,-1,2)),_xlpm.lower_xs,INDEX(_xlpm.xs,_xlpm.calc_idxs,1),_xlpm.upper_xs,INDEX(_xlpm.xs,_xlpm.calc_idxs+1,1),_xlpm.txs,(_xlpm.desired_xs-_xlpm.lower_xs)/(_xlpm.upper_xs-_xlpm.lower_xs),_xlpm.one_minus_txs,1-_xlpm.txs,_xlpm.lower_ys,INDEX(_xlpm.ys,_xlpm.calc_idxs,1),_xlpm.upper_ys,INDEX(_xlpm.ys,_xlpm.calc_idxs+1,1),_xlpm.ais,INDEX(_xlpm.as,_xlpm.calc_idxs,1),_xlpm.bis,INDEX(_xlpm.bs,_xlpm.calc_idxs,1),_xlpm.one_minus_txs*_xlpm.lower_ys+_xlpm.txs*_xlpm.upper_ys+_xlpm.txs*_xlpm.one_minus_txs*(_xlpm.one_minus_txs*_xlpm.ais+_xlpm.txs*_xlpm.bis)))</definedName>
     <definedName name="INTERNAL_SPLINE_MATRIX_TOP_BOTTOM">_xlfn.LAMBDA(_xlpm.end_type,_xlpm.row,_xlpm.col,_xlpm.recip_dxs,_xlpm.recip_dxs_sq,IF(_xlpm.end_type=0,_xlfn.LET(_xlpm.i,IF(_xlpm.row=1,1,_xlpm.row-1),_xlfn.IFS(_xlpm.row=_xlpm.col,2*INDEX(_xlpm.recip_dxs,_xlpm.i,1),OR(_xlpm.col=_xlpm.row+1,_xlpm.col=_xlpm.row-1),INDEX(_xlpm.recip_dxs,_xlpm.i,1),TRUE,0)),_xlfn.LET(_xlpm.c_start,IF(_xlpm.row=1,1,_xlpm.row-2),_xlpm.recip1,INDEX(_xlpm.recip_dxs_sq,_xlpm.c_start,1),_xlpm.recip2,INDEX(_xlpm.recip_dxs_sq,_xlpm.c_start+1,1),_xlfn.IFS(_xlpm.col=_xlpm.c_start,_xlpm.recip1,_xlpm.col=_xlpm.c_start+1,_xlpm.recip1-_xlpm.recip2,_xlpm.col=_xlpm.c_start+2,-_xlpm.recip2,TRUE,0))))</definedName>
     <definedName name="INTERNAL_SPLINE_VECTOR_TOP_BOTTOM">_xlfn.LAMBDA(_xlpm.end_type,_xlpm.row,_xlpm.recip_dxs,_xlpm.dys_recip_dxs_sq,IF(_xlpm.end_type=0,_xlfn.LET(_xlpm.i,IF(_xlpm.row=1,1,_xlpm.row-1),3*INDEX(_xlpm.dys_recip_dxs_sq,_xlpm.i,1)),_xlfn.LET(_xlpm.c_start,IF(_xlpm.row=1,1,_xlpm.row-2),_xlpm.recip1,INDEX(_xlpm.dys_recip_dxs_sq,_xlpm.c_start,1)*INDEX(_xlpm.recip_dxs,_xlpm.c_start,1),_xlpm.recip2,INDEX(_xlpm.dys_recip_dxs_sq,_xlpm.c_start+1,1)*INDEX(_xlpm.recip_dxs,_xlpm.c_start+1,1),2*(_xlpm.recip1-_xlpm.recip2))))</definedName>

</xml_diff>